<commit_message>
se completa compilador de escenarios
</commit_message>
<xml_diff>
--- a/test/test_inputs/Escenarios/Escenario_test1.xlsx
+++ b/test/test_inputs/Escenarios/Escenario_test1.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Trabajo\2022 - Demanda Electrica Coordinador\App\test\test_inputs\Escenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160653E4-D2DE-4A23-83AB-6971F0E5864B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D561CD-3FD8-4A1B-90C5-9096BB9333C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VarMensuales" sheetId="1" r:id="rId1"/>
-    <sheet name="Electromovilidad" sheetId="2" r:id="rId2"/>
+    <sheet name="Poblacion" sheetId="3" r:id="rId2"/>
+    <sheet name="Produccion" sheetId="4" r:id="rId3"/>
+    <sheet name="Electromovilidad" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Año</t>
   </si>
@@ -52,6 +54,21 @@
   </si>
   <si>
     <t>Precio</t>
+  </si>
+  <si>
+    <t>Comuna1</t>
+  </si>
+  <si>
+    <t>Comuna2</t>
+  </si>
+  <si>
+    <t>Empresa1</t>
+  </si>
+  <si>
+    <t>Empresa2</t>
+  </si>
+  <si>
+    <t>Empresa3</t>
   </si>
 </sst>
 </file>
@@ -371,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,6 +773,811 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75F1AC5-A15B-4319-A52D-D8E5716242BC}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2022</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2023</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2023</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2023</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2023</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2023</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2023</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2023</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2023</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2023</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C6FDD7-78E1-44D9-831D-1B1F4822FBC9}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2022</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2022</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2022</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2023</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2023</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2023</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2023</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2023</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2023</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2023</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2023</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2023</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2023</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC68B0B-280D-42D6-B441-1BDED65F8817}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>